<commit_message>
draw figure of K-Means
</commit_message>
<xml_diff>
--- a/OBD_project-master/OBD_GUI/KMeansData.xlsx
+++ b/OBD_project-master/OBD_GUI/KMeansData.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21601"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3ABF4421-AC14-49B7-8809-7960E7C606F7}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{10AA71FE-BFD1-40C6-87A3-F2E50D66AEE8}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="22932" yWindow="-108" windowWidth="23256" windowHeight="14016" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -27,12 +27,19 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="等线"/>
       <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <name val="等线"/>
+      <family val="3"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -60,7 +67,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="常规" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -338,15 +345,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D21"/>
+  <dimension ref="A1:D33"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F15" sqref="F15"/>
+      <selection activeCell="G25" sqref="G25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1">
         <v>0</v>
       </c>
@@ -360,7 +367,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>0</v>
       </c>
@@ -374,7 +381,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>0</v>
       </c>
@@ -388,7 +395,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>0.30147895335608643</v>
       </c>
@@ -402,7 +409,7 @@
         <v>0.33333333333333331</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>0.40896940896940898</v>
       </c>
@@ -416,7 +423,7 @@
         <v>0.45454545454545453</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>0.16956676136363638</v>
       </c>
@@ -430,7 +437,7 @@
         <v>0.15217391304347827</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>4.3360913965915363E-2</v>
       </c>
@@ -444,7 +451,7 @@
         <v>3.9215686274509803E-2</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>7.269097178935903E-2</v>
       </c>
@@ -458,7 +465,7 @@
         <v>9.0909090909090912E-2</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>0</v>
       </c>
@@ -472,7 +479,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>0</v>
       </c>
@@ -486,7 +493,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>4.0951913615612089E-2</v>
       </c>
@@ -500,7 +507,7 @@
         <v>4.0816326530612242E-2</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>1.2709116846064064E-2</v>
       </c>
@@ -514,7 +521,7 @@
         <v>3.125E-2</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>5.9049579687768063E-2</v>
       </c>
@@ -528,7 +535,7 @@
         <v>5.3333333333333337E-2</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>5.7411586293321465E-2</v>
       </c>
@@ -542,7 +549,7 @@
         <v>7.1428571428571425E-2</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>7.6940947063999177E-2</v>
       </c>
@@ -556,7 +563,7 @@
         <v>8.9552238805970144E-2</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>0.28921291339218957</v>
       </c>
@@ -570,7 +577,7 @@
         <v>0.33333333333333331</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>0.40699436676103079</v>
       </c>
@@ -584,7 +591,7 @@
         <v>0.43859649122807015</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>0.15269435870879189</v>
       </c>
@@ -598,7 +605,7 @@
         <v>0.21212121212121213</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>0.1590324877791959</v>
       </c>
@@ -612,7 +619,7 @@
         <v>0.21848739495798319</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>3.1462563585151551E-2</v>
       </c>
@@ -626,7 +633,7 @@
         <v>4.4776119402985072E-2</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>0</v>
       </c>
@@ -640,7 +647,176 @@
         <v>0</v>
       </c>
     </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A22">
+        <v>9.7759493033057754E-2</v>
+      </c>
+      <c r="B22">
+        <v>0.7857142857142857</v>
+      </c>
+      <c r="C22">
+        <v>9.5238095238095233E-2</v>
+      </c>
+      <c r="D22">
+        <v>0.11904761904761904</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A23">
+        <v>0.1403123154648645</v>
+      </c>
+      <c r="B23">
+        <v>0.74193548387096775</v>
+      </c>
+      <c r="C23">
+        <v>0</v>
+      </c>
+      <c r="D23">
+        <v>0.25806451612903225</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A24">
+        <v>9.9594668768384173E-2</v>
+      </c>
+      <c r="B24">
+        <v>0.77777777777777779</v>
+      </c>
+      <c r="C24">
+        <v>0</v>
+      </c>
+      <c r="D24">
+        <v>0.22222222222222221</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A25">
+        <v>7.2314177457176054E-2</v>
+      </c>
+      <c r="B25">
+        <v>0.7142857142857143</v>
+      </c>
+      <c r="C25">
+        <v>0.14285714285714285</v>
+      </c>
+      <c r="D25">
+        <v>0.14285714285714285</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A26">
+        <v>0.12815785436229221</v>
+      </c>
+      <c r="B26">
+        <v>0.5892857142857143</v>
+      </c>
+      <c r="C26">
+        <v>0.16071428571428573</v>
+      </c>
+      <c r="D26">
+        <v>0.25</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A27">
+        <v>0.22763461662938805</v>
+      </c>
+      <c r="B27">
+        <v>0.51063829787234039</v>
+      </c>
+      <c r="C27">
+        <v>0.10638297872340426</v>
+      </c>
+      <c r="D27">
+        <v>0.38297872340425532</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A28">
+        <v>7.6340388826538749E-2</v>
+      </c>
+      <c r="B28">
+        <v>0.67241379310344829</v>
+      </c>
+      <c r="C28">
+        <v>0.17241379310344829</v>
+      </c>
+      <c r="D28">
+        <v>0.15517241379310345</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A29">
+        <v>4.2110065951082826E-2</v>
+      </c>
+      <c r="B29">
+        <v>0.74576271186440679</v>
+      </c>
+      <c r="C29">
+        <v>0.16949152542372881</v>
+      </c>
+      <c r="D29">
+        <v>8.4745762711864403E-2</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A30">
+        <v>3.2417484929396438E-2</v>
+      </c>
+      <c r="B30">
+        <v>0.83333333333333337</v>
+      </c>
+      <c r="C30">
+        <v>0.1</v>
+      </c>
+      <c r="D30">
+        <v>6.6666666666666666E-2</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A31">
+        <v>2.2019603795038343E-2</v>
+      </c>
+      <c r="B31">
+        <v>0.84444444444444444</v>
+      </c>
+      <c r="C31">
+        <v>0.1111111111111111</v>
+      </c>
+      <c r="D31">
+        <v>4.4444444444444446E-2</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A32">
+        <v>6.6572544437592668E-2</v>
+      </c>
+      <c r="B32">
+        <v>0.39215686274509803</v>
+      </c>
+      <c r="C32">
+        <v>0.47058823529411764</v>
+      </c>
+      <c r="D32">
+        <v>0.13725490196078433</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A33">
+        <v>3.1628130371768516E-2</v>
+      </c>
+      <c r="B33">
+        <v>0.6071428571428571</v>
+      </c>
+      <c r="C33">
+        <v>0.32142857142857145</v>
+      </c>
+      <c r="D33">
+        <v>7.1428571428571425E-2</v>
+      </c>
+    </row>
   </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>